<commit_message>
module 4 & media updates
</commit_message>
<xml_diff>
--- a/materials_science_renderings/course_build_utilities/Planning Syllabus.xlsx
+++ b/materials_science_renderings/course_build_utilities/Planning Syllabus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://virginiatech.sharepoint.com/sites/SGCTeaching/Shared Documents/MSE_2034_D2L/vscode_brightspace_development/brightspace/materials_science_renderings/course_build_utilities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://virginiatech.sharepoint.com/sites/SGCTeaching/Shared Documents/MSE_2034_D2L/D2L_Master/brightspace/materials_science_renderings/course_build_utilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="503" documentId="8_{42A4FF08-CD82-40AF-A6ED-26AC52AD5C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD824C4C-DB86-43B5-8D2A-38A4CF779846}"/>
+  <xr:revisionPtr revIDLastSave="512" documentId="8_{42A4FF08-CD82-40AF-A6ED-26AC52AD5C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A6008D0-AF35-4125-9060-E73BF827A934}"/>
   <bookViews>
-    <workbookView xWindow="-18105" yWindow="0" windowWidth="18210" windowHeight="14145" activeTab="1" xr2:uid="{E8C7E3EB-A789-47ED-AC38-4781AECB45EE}"/>
+    <workbookView xWindow="-17385" yWindow="1560" windowWidth="16830" windowHeight="23010" activeTab="1" xr2:uid="{E8C7E3EB-A789-47ED-AC38-4781AECB45EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Fall MWF Mon start" sheetId="2" r:id="rId1"/>
@@ -1071,6 +1071,93 @@
     <xf numFmtId="165" fontId="2" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1116,12 +1203,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1131,60 +1212,6 @@
     <xf numFmtId="165" fontId="2" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1194,61 +1221,34 @@
     <xf numFmtId="165" fontId="2" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1275,10 +1275,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1599,11 +1595,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="94">
+      <c r="C1" s="50"/>
+      <c r="D1" s="56">
         <v>45530</v>
       </c>
       <c r="E1" s="13" t="s">
@@ -1613,48 +1609,48 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="2:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="94"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="56"/>
     </row>
     <row r="3" spans="2:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="94"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="93"/>
+      <c r="C4" s="55"/>
       <c r="D4" s="7">
         <v>45642</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="93"/>
+      <c r="C5" s="55"/>
       <c r="D5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
     </row>
     <row r="6" spans="2:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="95" t="s">
+      <c r="E6" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="96"/>
+      <c r="F6" s="58"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1685,7 +1681,7 @@
       </c>
     </row>
     <row r="8" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="65">
+      <c r="B8" s="52">
         <v>1</v>
       </c>
       <c r="C8" s="20">
@@ -1695,15 +1691,15 @@
         <f>D1</f>
         <v>45530</v>
       </c>
-      <c r="E8" s="97" t="s">
+      <c r="E8" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="99" t="s">
+      <c r="F8" s="61" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="70"/>
+      <c r="B9" s="53"/>
       <c r="C9" s="18">
         <v>2</v>
       </c>
@@ -1711,11 +1707,11 @@
         <f>D8+2</f>
         <v>45532</v>
       </c>
-      <c r="E9" s="98"/>
-      <c r="F9" s="71"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="62"/>
     </row>
     <row r="10" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="78"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="23">
         <v>3</v>
       </c>
@@ -1723,16 +1719,16 @@
         <f>D9+2</f>
         <v>45534</v>
       </c>
-      <c r="E10" s="98"/>
-      <c r="F10" s="71"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="62"/>
     </row>
     <row r="11" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="72">
+      <c r="B11" s="73">
         <f>D8+7</f>
         <v>45537</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="75"/>
       <c r="E11" s="28" t="s">
         <v>16</v>
       </c>
@@ -1744,7 +1740,7 @@
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="65">
+      <c r="B12" s="52">
         <v>2</v>
       </c>
       <c r="C12" s="20">
@@ -1754,15 +1750,15 @@
         <f t="shared" ref="D12:D54" si="0">D9+7</f>
         <v>45539</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="E12" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="71" t="s">
+      <c r="F12" s="62" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="70"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="18">
         <v>5</v>
       </c>
@@ -1770,11 +1766,11 @@
         <f t="shared" si="0"/>
         <v>45541</v>
       </c>
-      <c r="E13" s="70"/>
-      <c r="F13" s="71"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="62"/>
     </row>
     <row r="14" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="81">
+      <c r="B14" s="65">
         <v>3</v>
       </c>
       <c r="C14" s="20">
@@ -1784,15 +1780,15 @@
         <f>B11+7</f>
         <v>45544</v>
       </c>
-      <c r="E14" s="66" t="s">
+      <c r="E14" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="85" t="s">
+      <c r="F14" s="70" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="82"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="18">
         <v>7</v>
       </c>
@@ -1800,11 +1796,11 @@
         <f t="shared" si="0"/>
         <v>45546</v>
       </c>
-      <c r="E15" s="82"/>
-      <c r="F15" s="86"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="71"/>
     </row>
     <row r="16" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="83"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="23">
         <v>8</v>
       </c>
@@ -1812,11 +1808,11 @@
         <f t="shared" si="0"/>
         <v>45548</v>
       </c>
-      <c r="E16" s="84"/>
-      <c r="F16" s="87"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="72"/>
     </row>
     <row r="17" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="65">
+      <c r="B17" s="52">
         <v>4</v>
       </c>
       <c r="C17" s="20">
@@ -1826,15 +1822,15 @@
         <f t="shared" si="0"/>
         <v>45551</v>
       </c>
-      <c r="E17" s="70" t="s">
+      <c r="E17" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="71" t="s">
+      <c r="F17" s="62" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="70"/>
+      <c r="B18" s="53"/>
       <c r="C18" s="18">
         <v>10</v>
       </c>
@@ -1842,11 +1838,11 @@
         <f t="shared" si="0"/>
         <v>45553</v>
       </c>
-      <c r="E18" s="70"/>
-      <c r="F18" s="71"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="62"/>
     </row>
     <row r="19" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="78"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="23">
         <v>11</v>
       </c>
@@ -1854,11 +1850,11 @@
         <f t="shared" si="0"/>
         <v>45555</v>
       </c>
-      <c r="E19" s="70"/>
-      <c r="F19" s="71"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="62"/>
     </row>
     <row r="20" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="65">
+      <c r="B20" s="52">
         <v>5</v>
       </c>
       <c r="C20" s="20">
@@ -1868,15 +1864,15 @@
         <f t="shared" si="0"/>
         <v>45558</v>
       </c>
-      <c r="E20" s="70" t="s">
+      <c r="E20" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="71" t="s">
+      <c r="F20" s="62" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="70"/>
+      <c r="B21" s="53"/>
       <c r="C21" s="18">
         <v>13</v>
       </c>
@@ -1884,11 +1880,11 @@
         <f t="shared" si="0"/>
         <v>45560</v>
       </c>
-      <c r="E21" s="70"/>
-      <c r="F21" s="71"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="62"/>
     </row>
     <row r="22" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="78"/>
+      <c r="B22" s="54"/>
       <c r="C22" s="23">
         <v>14</v>
       </c>
@@ -1896,11 +1892,11 @@
         <f t="shared" si="0"/>
         <v>45562</v>
       </c>
-      <c r="E22" s="70"/>
-      <c r="F22" s="71"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="62"/>
     </row>
     <row r="23" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="65">
+      <c r="B23" s="52">
         <v>6</v>
       </c>
       <c r="C23" s="20">
@@ -1910,15 +1906,15 @@
         <f t="shared" si="0"/>
         <v>45565</v>
       </c>
-      <c r="E23" s="70" t="s">
+      <c r="E23" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="71" t="s">
+      <c r="F23" s="62" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="70"/>
+      <c r="B24" s="53"/>
       <c r="C24" s="18">
         <v>16</v>
       </c>
@@ -1926,11 +1922,11 @@
         <f t="shared" si="0"/>
         <v>45567</v>
       </c>
-      <c r="E24" s="70"/>
-      <c r="F24" s="71"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="62"/>
     </row>
     <row r="25" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="78"/>
+      <c r="B25" s="54"/>
       <c r="C25" s="23">
         <v>17</v>
       </c>
@@ -1938,11 +1934,11 @@
         <f t="shared" si="0"/>
         <v>45569</v>
       </c>
-      <c r="E25" s="70"/>
-      <c r="F25" s="71"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="62"/>
     </row>
     <row r="26" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="65">
+      <c r="B26" s="52">
         <v>7</v>
       </c>
       <c r="C26" s="20">
@@ -1952,15 +1948,15 @@
         <f t="shared" si="0"/>
         <v>45572</v>
       </c>
-      <c r="E26" s="70" t="s">
+      <c r="E26" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="71" t="s">
+      <c r="F26" s="62" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="70"/>
+      <c r="B27" s="53"/>
       <c r="C27" s="18">
         <v>19</v>
       </c>
@@ -1968,16 +1964,16 @@
         <f t="shared" si="0"/>
         <v>45574</v>
       </c>
-      <c r="E27" s="70"/>
-      <c r="F27" s="71"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="62"/>
     </row>
     <row r="28" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="72">
+      <c r="B28" s="73">
         <f>D25+7</f>
         <v>45576</v>
       </c>
-      <c r="C28" s="73"/>
-      <c r="D28" s="74"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="75"/>
       <c r="E28" s="28" t="s">
         <v>17</v>
       </c>
@@ -1989,7 +1985,7 @@
       <c r="K28" s="12"/>
     </row>
     <row r="29" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="65">
+      <c r="B29" s="52">
         <v>8</v>
       </c>
       <c r="C29" s="20">
@@ -1999,15 +1995,15 @@
         <f t="shared" si="0"/>
         <v>45579</v>
       </c>
-      <c r="E29" s="70" t="s">
+      <c r="E29" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="F29" s="71" t="s">
+      <c r="F29" s="62" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="30" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="70"/>
+      <c r="B30" s="53"/>
       <c r="C30" s="18">
         <v>21</v>
       </c>
@@ -2015,11 +2011,11 @@
         <f t="shared" si="0"/>
         <v>45581</v>
       </c>
-      <c r="E30" s="70"/>
-      <c r="F30" s="71"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="62"/>
     </row>
     <row r="31" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="78"/>
+      <c r="B31" s="54"/>
       <c r="C31" s="23">
         <v>22</v>
       </c>
@@ -2027,11 +2023,11 @@
         <f>B28+7</f>
         <v>45583</v>
       </c>
-      <c r="E31" s="70"/>
-      <c r="F31" s="71"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="62"/>
     </row>
     <row r="32" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="65">
+      <c r="B32" s="52">
         <v>9</v>
       </c>
       <c r="C32" s="20">
@@ -2041,15 +2037,15 @@
         <f t="shared" si="0"/>
         <v>45586</v>
       </c>
-      <c r="E32" s="70" t="s">
+      <c r="E32" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="71" t="s">
+      <c r="F32" s="62" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="33" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="70"/>
+      <c r="B33" s="53"/>
       <c r="C33" s="18">
         <v>24</v>
       </c>
@@ -2057,11 +2053,11 @@
         <f t="shared" si="0"/>
         <v>45588</v>
       </c>
-      <c r="E33" s="70"/>
-      <c r="F33" s="71"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="62"/>
     </row>
     <row r="34" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="78"/>
+      <c r="B34" s="54"/>
       <c r="C34" s="23">
         <v>25</v>
       </c>
@@ -2069,11 +2065,11 @@
         <f t="shared" si="0"/>
         <v>45590</v>
       </c>
-      <c r="E34" s="70"/>
-      <c r="F34" s="71"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="62"/>
     </row>
     <row r="35" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="65">
+      <c r="B35" s="52">
         <v>10</v>
       </c>
       <c r="C35" s="20">
@@ -2083,15 +2079,15 @@
         <f t="shared" si="0"/>
         <v>45593</v>
       </c>
-      <c r="E35" s="79" t="s">
+      <c r="E35" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="80" t="s">
+      <c r="F35" s="64" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="36" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="70"/>
+      <c r="B36" s="53"/>
       <c r="C36" s="18">
         <v>27</v>
       </c>
@@ -2099,11 +2095,11 @@
         <f t="shared" si="0"/>
         <v>45595</v>
       </c>
-      <c r="E36" s="70"/>
-      <c r="F36" s="71"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="62"/>
     </row>
     <row r="37" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="78"/>
+      <c r="B37" s="54"/>
       <c r="C37" s="23">
         <v>28</v>
       </c>
@@ -2111,11 +2107,11 @@
         <f t="shared" si="0"/>
         <v>45597</v>
       </c>
-      <c r="E37" s="70"/>
-      <c r="F37" s="71"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="62"/>
     </row>
     <row r="38" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="65">
+      <c r="B38" s="52">
         <v>11</v>
       </c>
       <c r="C38" s="20">
@@ -2125,15 +2121,15 @@
         <f t="shared" si="0"/>
         <v>45600</v>
       </c>
-      <c r="E38" s="70" t="s">
+      <c r="E38" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="F38" s="71" t="s">
+      <c r="F38" s="62" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="39" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="70"/>
+      <c r="B39" s="53"/>
       <c r="C39" s="18">
         <v>30</v>
       </c>
@@ -2141,11 +2137,11 @@
         <f t="shared" si="0"/>
         <v>45602</v>
       </c>
-      <c r="E39" s="70"/>
-      <c r="F39" s="71"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="62"/>
     </row>
     <row r="40" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="78"/>
+      <c r="B40" s="54"/>
       <c r="C40" s="23">
         <v>31</v>
       </c>
@@ -2153,11 +2149,11 @@
         <f t="shared" si="0"/>
         <v>45604</v>
       </c>
-      <c r="E40" s="70"/>
-      <c r="F40" s="71"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="62"/>
     </row>
     <row r="41" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="65">
+      <c r="B41" s="52">
         <v>12</v>
       </c>
       <c r="C41" s="20">
@@ -2167,15 +2163,15 @@
         <f t="shared" si="0"/>
         <v>45607</v>
       </c>
-      <c r="E41" s="70" t="s">
+      <c r="E41" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="F41" s="71" t="s">
+      <c r="F41" s="62" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="42" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="70"/>
+      <c r="B42" s="53"/>
       <c r="C42" s="18">
         <v>33</v>
       </c>
@@ -2183,11 +2179,11 @@
         <f t="shared" si="0"/>
         <v>45609</v>
       </c>
-      <c r="E42" s="70"/>
-      <c r="F42" s="71"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="62"/>
     </row>
     <row r="43" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="78"/>
+      <c r="B43" s="54"/>
       <c r="C43" s="23">
         <v>34</v>
       </c>
@@ -2195,11 +2191,11 @@
         <f t="shared" si="0"/>
         <v>45611</v>
       </c>
-      <c r="E43" s="70"/>
-      <c r="F43" s="71"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="62"/>
     </row>
     <row r="44" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="65">
+      <c r="B44" s="52">
         <v>13</v>
       </c>
       <c r="C44" s="20">
@@ -2209,15 +2205,15 @@
         <f t="shared" si="0"/>
         <v>45614</v>
       </c>
-      <c r="E44" s="70" t="s">
+      <c r="E44" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="F44" s="71" t="s">
+      <c r="F44" s="62" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="45" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="70"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="18">
         <v>36</v>
       </c>
@@ -2225,11 +2221,11 @@
         <f t="shared" si="0"/>
         <v>45616</v>
       </c>
-      <c r="E45" s="70"/>
-      <c r="F45" s="71"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="62"/>
     </row>
     <row r="46" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="78"/>
+      <c r="B46" s="54"/>
       <c r="C46" s="23">
         <v>37</v>
       </c>
@@ -2237,20 +2233,20 @@
         <f t="shared" si="0"/>
         <v>45618</v>
       </c>
-      <c r="E46" s="70"/>
-      <c r="F46" s="71"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="62"/>
     </row>
     <row r="47" spans="2:11" ht="15.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="75">
+      <c r="B47" s="76">
         <f>D44+7</f>
         <v>45621</v>
       </c>
-      <c r="C47" s="76"/>
-      <c r="D47" s="77"/>
-      <c r="E47" s="50" t="s">
+      <c r="C47" s="77"/>
+      <c r="D47" s="78"/>
+      <c r="E47" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="F47" s="53"/>
+      <c r="F47" s="82"/>
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
       <c r="I47" s="12"/>
@@ -2258,14 +2254,14 @@
       <c r="K47" s="12"/>
     </row>
     <row r="48" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="67">
+      <c r="B48" s="94">
         <f>D45+7</f>
         <v>45623</v>
       </c>
-      <c r="C48" s="68"/>
-      <c r="D48" s="69"/>
-      <c r="E48" s="51"/>
-      <c r="F48" s="54"/>
+      <c r="C48" s="95"/>
+      <c r="D48" s="96"/>
+      <c r="E48" s="80"/>
+      <c r="F48" s="83"/>
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
@@ -2273,14 +2269,14 @@
       <c r="K48" s="12"/>
     </row>
     <row r="49" spans="2:11" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="88">
+      <c r="B49" s="97">
         <f>D46+7</f>
         <v>45625</v>
       </c>
-      <c r="C49" s="89"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="52"/>
-      <c r="F49" s="55"/>
+      <c r="C49" s="98"/>
+      <c r="D49" s="99"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="84"/>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
@@ -2288,7 +2284,7 @@
       <c r="K49" s="12"/>
     </row>
     <row r="50" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="65">
+      <c r="B50" s="52">
         <v>14</v>
       </c>
       <c r="C50" s="20">
@@ -2298,15 +2294,15 @@
         <f>B47+7</f>
         <v>45628</v>
       </c>
-      <c r="E50" s="70" t="s">
+      <c r="E50" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="F50" s="71" t="s">
+      <c r="F50" s="62" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="51" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="70"/>
+      <c r="B51" s="53"/>
       <c r="C51" s="18">
         <v>39</v>
       </c>
@@ -2314,11 +2310,11 @@
         <f>B48+7</f>
         <v>45630</v>
       </c>
-      <c r="E51" s="70"/>
-      <c r="F51" s="71"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="62"/>
     </row>
     <row r="52" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="78"/>
+      <c r="B52" s="54"/>
       <c r="C52" s="23">
         <v>40</v>
       </c>
@@ -2326,11 +2322,11 @@
         <f>B49+7</f>
         <v>45632</v>
       </c>
-      <c r="E52" s="70"/>
-      <c r="F52" s="71"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="62"/>
     </row>
     <row r="53" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="65">
+      <c r="B53" s="52">
         <v>15</v>
       </c>
       <c r="C53" s="20">
@@ -2340,13 +2336,13 @@
         <f t="shared" si="0"/>
         <v>45635</v>
       </c>
-      <c r="E53" s="70" t="s">
+      <c r="E53" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F53" s="71"/>
+      <c r="F53" s="62"/>
     </row>
     <row r="54" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="66"/>
+      <c r="B54" s="68"/>
       <c r="C54" s="19">
         <v>42</v>
       </c>
@@ -2354,16 +2350,16 @@
         <f t="shared" si="0"/>
         <v>45637</v>
       </c>
-      <c r="E54" s="70"/>
-      <c r="F54" s="71"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="62"/>
     </row>
     <row r="55" spans="2:11" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="56">
+      <c r="B55" s="85">
         <f>D52+6</f>
         <v>45638</v>
       </c>
-      <c r="C55" s="57"/>
-      <c r="D55" s="58"/>
+      <c r="C55" s="86"/>
+      <c r="D55" s="87"/>
       <c r="E55" s="31" t="s">
         <v>19</v>
       </c>
@@ -2375,19 +2371,19 @@
       <c r="K55" s="12"/>
     </row>
     <row r="56" spans="2:11" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="62"/>
-      <c r="C56" s="63"/>
-      <c r="D56" s="64"/>
+      <c r="B56" s="91"/>
+      <c r="C56" s="92"/>
+      <c r="D56" s="93"/>
       <c r="E56" s="17"/>
       <c r="F56" s="33"/>
     </row>
     <row r="57" spans="2:11" ht="14.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="59">
+      <c r="B57" s="88">
         <f>D4</f>
         <v>45642</v>
       </c>
-      <c r="C57" s="60"/>
-      <c r="D57" s="61">
+      <c r="C57" s="89"/>
+      <c r="D57" s="90">
         <f>D4</f>
         <v>45642</v>
       </c>
@@ -2409,30 +2405,28 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="B1:C3"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B46"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="E44:E46"/>
@@ -2449,28 +2443,30 @@
     <mergeCell ref="F38:F40"/>
     <mergeCell ref="E41:E43"/>
     <mergeCell ref="F41:F43"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B1:C3"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2481,11 +2477,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5554DA7D-267F-460B-9BA9-EA602D83332F}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C60" sqref="C60"/>
+      <selection pane="bottomRight" activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2502,10 +2498,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="91"/>
+      <c r="B1" s="50"/>
       <c r="C1" s="7">
         <v>45679</v>
       </c>
@@ -2520,8 +2516,8 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="91"/>
-      <c r="B2" s="91"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
       <c r="C2" s="7"/>
       <c r="E2" s="9" t="s">
         <v>8</v>
@@ -2534,22 +2530,22 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="91"/>
-      <c r="B3" s="91"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
       <c r="C3" s="7"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D5" s="92" t="s">
+      <c r="D5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="92" t="s">
+      <c r="H5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
@@ -2580,7 +2576,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="103">
+      <c r="A7" s="109">
         <v>1</v>
       </c>
       <c r="B7" s="4">
@@ -2595,7 +2591,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="103"/>
+      <c r="A8" s="109"/>
       <c r="B8" s="4">
         <v>2</v>
       </c>
@@ -2608,7 +2604,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="100">
+      <c r="A9" s="106">
         <v>2</v>
       </c>
       <c r="B9" s="35">
@@ -2630,7 +2626,7 @@
       <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="101"/>
+      <c r="A10" s="107"/>
       <c r="B10" s="4">
         <v>4</v>
       </c>
@@ -2644,7 +2640,7 @@
       <c r="K10" s="39"/>
     </row>
     <row r="11" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="102"/>
+      <c r="A11" s="108"/>
       <c r="B11" s="40">
         <v>5</v>
       </c>
@@ -2664,7 +2660,7 @@
       <c r="K11" s="43"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="103">
+      <c r="A12" s="109">
         <v>3</v>
       </c>
       <c r="B12" s="4">
@@ -2679,7 +2675,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="103"/>
+      <c r="A13" s="109"/>
       <c r="B13" s="4">
         <v>7</v>
       </c>
@@ -2692,7 +2688,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="103"/>
+      <c r="A14" s="109"/>
       <c r="B14" s="4">
         <v>8</v>
       </c>
@@ -2705,7 +2701,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="100">
+      <c r="A15" s="106">
         <v>4</v>
       </c>
       <c r="B15" s="35">
@@ -2727,7 +2723,7 @@
       <c r="K15" s="38"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="101"/>
+      <c r="A16" s="107"/>
       <c r="B16" s="4">
         <v>10</v>
       </c>
@@ -2741,7 +2737,7 @@
       <c r="K16" s="39"/>
     </row>
     <row r="17" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="102"/>
+      <c r="A17" s="108"/>
       <c r="B17" s="40">
         <v>11</v>
       </c>
@@ -2761,7 +2757,7 @@
       <c r="K17" s="43"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="103">
+      <c r="A18" s="109">
         <v>5</v>
       </c>
       <c r="B18" s="4">
@@ -2776,7 +2772,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="103"/>
+      <c r="A19" s="109"/>
       <c r="B19" s="4">
         <v>13</v>
       </c>
@@ -2789,7 +2785,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="103"/>
+      <c r="A20" s="109"/>
       <c r="B20" s="4">
         <v>14</v>
       </c>
@@ -2802,7 +2798,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="100">
+      <c r="A21" s="106">
         <v>6</v>
       </c>
       <c r="B21" s="35">
@@ -2824,7 +2820,7 @@
       <c r="K21" s="38"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="101"/>
+      <c r="A22" s="107"/>
       <c r="B22" s="4">
         <v>16</v>
       </c>
@@ -2838,7 +2834,7 @@
       <c r="K22" s="39"/>
     </row>
     <row r="23" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="102"/>
+      <c r="A23" s="108"/>
       <c r="B23" s="40">
         <v>17</v>
       </c>
@@ -2858,7 +2854,7 @@
       <c r="K23" s="43"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="103">
+      <c r="A24" s="109">
         <v>7</v>
       </c>
       <c r="B24" s="4">
@@ -2873,7 +2869,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="103"/>
+      <c r="A25" s="109"/>
       <c r="B25" s="4">
         <v>19</v>
       </c>
@@ -2886,7 +2882,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="103"/>
+      <c r="A26" s="109"/>
       <c r="B26" s="4">
         <v>20</v>
       </c>
@@ -2905,16 +2901,16 @@
         <f t="shared" si="1"/>
         <v>45726</v>
       </c>
-      <c r="D27" s="104" t="s">
+      <c r="D27" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="104"/>
-      <c r="F27" s="104"/>
-      <c r="G27" s="104"/>
-      <c r="H27" s="104"/>
-      <c r="I27" s="104"/>
-      <c r="J27" s="104"/>
-      <c r="K27" s="105"/>
+      <c r="E27" s="100"/>
+      <c r="F27" s="100"/>
+      <c r="G27" s="100"/>
+      <c r="H27" s="100"/>
+      <c r="I27" s="100"/>
+      <c r="J27" s="100"/>
+      <c r="K27" s="101"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="111"/>
@@ -2923,14 +2919,14 @@
         <f t="shared" si="1"/>
         <v>45728</v>
       </c>
-      <c r="D28" s="106"/>
-      <c r="E28" s="106"/>
-      <c r="F28" s="106"/>
-      <c r="G28" s="106"/>
-      <c r="H28" s="106"/>
-      <c r="I28" s="106"/>
-      <c r="J28" s="106"/>
-      <c r="K28" s="107"/>
+      <c r="D28" s="102"/>
+      <c r="E28" s="102"/>
+      <c r="F28" s="102"/>
+      <c r="G28" s="102"/>
+      <c r="H28" s="102"/>
+      <c r="I28" s="102"/>
+      <c r="J28" s="102"/>
+      <c r="K28" s="103"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="112"/>
@@ -2939,17 +2935,17 @@
         <f t="shared" si="1"/>
         <v>45730</v>
       </c>
-      <c r="D29" s="108"/>
-      <c r="E29" s="108"/>
-      <c r="F29" s="108"/>
-      <c r="G29" s="108"/>
-      <c r="H29" s="108"/>
-      <c r="I29" s="108"/>
-      <c r="J29" s="108"/>
-      <c r="K29" s="109"/>
+      <c r="D29" s="104"/>
+      <c r="E29" s="104"/>
+      <c r="F29" s="104"/>
+      <c r="G29" s="104"/>
+      <c r="H29" s="104"/>
+      <c r="I29" s="104"/>
+      <c r="J29" s="104"/>
+      <c r="K29" s="105"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="103">
+      <c r="A30" s="109">
         <v>8</v>
       </c>
       <c r="B30" s="4">
@@ -2964,7 +2960,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="103"/>
+      <c r="A31" s="109"/>
       <c r="B31" s="4">
         <v>22</v>
       </c>
@@ -2977,7 +2973,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="103"/>
+      <c r="A32" s="109"/>
       <c r="B32" s="4">
         <v>23</v>
       </c>
@@ -2990,7 +2986,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="100">
+      <c r="A33" s="106">
         <v>9</v>
       </c>
       <c r="B33" s="35">
@@ -3012,7 +3008,7 @@
       <c r="K33" s="38"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="101"/>
+      <c r="A34" s="107"/>
       <c r="B34" s="4">
         <v>25</v>
       </c>
@@ -3026,7 +3022,7 @@
       <c r="K34" s="39"/>
     </row>
     <row r="35" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="102"/>
+      <c r="A35" s="108"/>
       <c r="B35" s="40">
         <v>26</v>
       </c>
@@ -3046,7 +3042,7 @@
       <c r="K35" s="43"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="103">
+      <c r="A36" s="109">
         <v>10</v>
       </c>
       <c r="B36" s="4">
@@ -3061,7 +3057,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="103"/>
+      <c r="A37" s="109"/>
       <c r="B37" s="4">
         <v>28</v>
       </c>
@@ -3074,7 +3070,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="103"/>
+      <c r="A38" s="109"/>
       <c r="B38" s="4">
         <v>29</v>
       </c>
@@ -3087,7 +3083,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="100">
+      <c r="A39" s="106">
         <v>11</v>
       </c>
       <c r="B39" s="35">
@@ -3109,7 +3105,7 @@
       <c r="K39" s="38"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="101"/>
+      <c r="A40" s="107"/>
       <c r="B40" s="4">
         <v>31</v>
       </c>
@@ -3123,7 +3119,7 @@
       <c r="K40" s="39"/>
     </row>
     <row r="41" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="102"/>
+      <c r="A41" s="108"/>
       <c r="B41" s="40">
         <v>32</v>
       </c>
@@ -3143,7 +3139,7 @@
       <c r="K41" s="43"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="103">
+      <c r="A42" s="109">
         <v>12</v>
       </c>
       <c r="B42" s="4">
@@ -3158,7 +3154,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="103"/>
+      <c r="A43" s="109"/>
       <c r="B43" s="4">
         <v>34</v>
       </c>
@@ -3171,7 +3167,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="103"/>
+      <c r="A44" s="109"/>
       <c r="B44" s="4">
         <v>35</v>
       </c>
@@ -3184,7 +3180,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="100">
+      <c r="A45" s="106">
         <v>13</v>
       </c>
       <c r="B45" s="35">
@@ -3206,7 +3202,7 @@
       <c r="K45" s="38"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="101"/>
+      <c r="A46" s="107"/>
       <c r="B46" s="4">
         <v>37</v>
       </c>
@@ -3220,7 +3216,7 @@
       <c r="K46" s="39"/>
     </row>
     <row r="47" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="102"/>
+      <c r="A47" s="108"/>
       <c r="B47" s="40">
         <v>38</v>
       </c>
@@ -3240,7 +3236,7 @@
       <c r="K47" s="43"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="103">
+      <c r="A48" s="109">
         <v>14</v>
       </c>
       <c r="B48" s="4">
@@ -3255,7 +3251,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="103"/>
+      <c r="A49" s="109"/>
       <c r="B49" s="4">
         <v>40</v>
       </c>
@@ -3268,7 +3264,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="103"/>
+      <c r="A50" s="109"/>
       <c r="B50" s="4">
         <v>41</v>
       </c>
@@ -3281,7 +3277,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="100">
+      <c r="A51" s="106">
         <v>15</v>
       </c>
       <c r="B51" s="35">
@@ -3303,7 +3299,7 @@
       <c r="K51" s="38"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="101"/>
+      <c r="A52" s="107"/>
       <c r="B52" s="4">
         <v>43</v>
       </c>
@@ -3318,14 +3314,21 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C54" s="7"/>
-      <c r="D54" s="92" t="s">
+      <c r="D54" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="E54" s="92"/>
-      <c r="F54" s="92"/>
+      <c r="E54" s="51"/>
+      <c r="F54" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
     <mergeCell ref="D27:K29"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="A51:A52"/>
@@ -3340,41 +3343,15 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1" gridLines="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
+  <pageSetup scale="75" fitToWidth="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0ffa7682-a752-4ec2-9b00-944c9a00bbe9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5bbddf2c-15bd-4cee-88ee-4bb358fdb5d4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100140A42B38915AC4EBAF791562DC92B4E" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="45dcb3ee8ab16e94e9ce11f52f3ef1c8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5bbddf2c-15bd-4cee-88ee-4bb358fdb5d4" xmlns:ns3="0ffa7682-a752-4ec2-9b00-944c9a00bbe9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ee4a90daa14cdc5725b57d2c9b788eb1" ns2:_="" ns3:_="">
     <xsd:import namespace="5bbddf2c-15bd-4cee-88ee-4bb358fdb5d4"/>
@@ -3581,13 +3558,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0ffa7682-a752-4ec2-9b00-944c9a00bbe9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5bbddf2c-15bd-4cee-88ee-4bb358fdb5d4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{292990A1-DB53-45B6-B715-CD9972EFC688}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{572559A9-8F66-4BA8-9CA2-4F0B96392493}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5bbddf2c-15bd-4cee-88ee-4bb358fdb5d4"/>
+    <ds:schemaRef ds:uri="0ffa7682-a752-4ec2-9b00-944c9a00bbe9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0ffa7682-a752-4ec2-9b00-944c9a00bbe9"/>
-    <ds:schemaRef ds:uri="5bbddf2c-15bd-4cee-88ee-4bb358fdb5d4"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3601,5 +3606,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{572559A9-8F66-4BA8-9CA2-4F0B96392493}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{292990A1-DB53-45B6-B715-CD9972EFC688}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0ffa7682-a752-4ec2-9b00-944c9a00bbe9"/>
+    <ds:schemaRef ds:uri="5bbddf2c-15bd-4cee-88ee-4bb358fdb5d4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>